<commit_message>
Actualizacion mapa y base de rutas
</commit_message>
<xml_diff>
--- a/CronogramaProyecto.xlsx
+++ b/CronogramaProyecto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\landm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7533855fb1921b0c/Escritorio/DesarrolloProyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9EED57-0BCF-491D-B0AC-B47665181D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{3A9EED57-0BCF-491D-B0AC-B47665181D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF97288C-FA6D-44BE-8367-95E1E8B6395C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma de proyecto simple" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t>Tom</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Sofia, Jan</t>
+  </si>
+  <si>
+    <t>Realizada</t>
+  </si>
+  <si>
+    <t>En proceso de Verificacion</t>
   </si>
 </sst>
 </file>
@@ -1926,43 +1932,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1970,7 +1976,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4702,6 +4708,10 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6224,8 +6234,8 @@
   </sheetPr>
   <dimension ref="B1:J43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6315,7 +6325,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>70</v>
@@ -6341,7 +6351,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>71</v>
@@ -6387,7 +6397,7 @@
         <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>72</v>
@@ -6413,7 +6423,7 @@
         <v>46</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>73</v>
@@ -6439,7 +6449,7 @@
         <v>47</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>71</v>
@@ -6485,7 +6495,7 @@
         <v>61</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>72</v>
@@ -6511,7 +6521,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>73</v>
@@ -6537,7 +6547,7 @@
         <v>63</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>71</v>
@@ -6994,18 +7004,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="57" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="57" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000Gantt Chart_x000D_</oddHeader>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3073" r:id="rId3" name="Check Box 1">
+            <control shapeId="3073" r:id="rId4" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7027,7 +7037,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3074" r:id="rId4" name="Check Box 2">
+            <control shapeId="3074" r:id="rId5" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7049,7 +7059,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3075" r:id="rId5" name="Check Box 3">
+            <control shapeId="3075" r:id="rId6" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7071,7 +7081,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3076" r:id="rId6" name="Check Box 4">
+            <control shapeId="3076" r:id="rId7" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7093,7 +7103,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3077" r:id="rId7" name="Check Box 5">
+            <control shapeId="3077" r:id="rId8" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7115,7 +7125,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3078" r:id="rId8" name="Check Box 6">
+            <control shapeId="3078" r:id="rId9" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7137,7 +7147,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3079" r:id="rId9" name="Check Box 7">
+            <control shapeId="3079" r:id="rId10" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7159,7 +7169,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3080" r:id="rId10" name="Check Box 8">
+            <control shapeId="3080" r:id="rId11" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7181,7 +7191,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3081" r:id="rId11" name="Check Box 9">
+            <control shapeId="3081" r:id="rId12" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7203,7 +7213,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3082" r:id="rId12" name="Check Box 10">
+            <control shapeId="3082" r:id="rId13" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7225,7 +7235,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3083" r:id="rId13" name="Check Box 11">
+            <control shapeId="3083" r:id="rId14" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7247,7 +7257,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3084" r:id="rId14" name="Check Box 12">
+            <control shapeId="3084" r:id="rId15" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7269,7 +7279,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3085" r:id="rId15" name="Check Box 13">
+            <control shapeId="3085" r:id="rId16" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7291,7 +7301,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3086" r:id="rId16" name="Check Box 14">
+            <control shapeId="3086" r:id="rId17" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7313,7 +7323,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3087" r:id="rId17" name="Check Box 15">
+            <control shapeId="3087" r:id="rId18" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7335,7 +7345,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3088" r:id="rId18" name="Check Box 16">
+            <control shapeId="3088" r:id="rId19" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7357,7 +7367,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3089" r:id="rId19" name="Check Box 17">
+            <control shapeId="3089" r:id="rId20" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7379,7 +7389,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3090" r:id="rId20" name="Check Box 18">
+            <control shapeId="3090" r:id="rId21" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -7401,7 +7411,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3091" r:id="rId21" name="Check Box 19">
+            <control shapeId="3091" r:id="rId22" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>

<commit_message>
Solucion de errores recientes y tamano frame 2
</commit_message>
<xml_diff>
--- a/CronogramaProyecto.xlsx
+++ b/CronogramaProyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7533855fb1921b0c/Escritorio/DesarrolloProyecto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{3A9EED57-0BCF-491D-B0AC-B47665181D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF97288C-FA6D-44BE-8367-95E1E8B6395C}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{3A9EED57-0BCF-491D-B0AC-B47665181D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51523E94-82F2-46E3-80A0-BF9B79420794}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11835" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma de proyecto simple" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1980,35 +1980,35 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6234,8 +6234,8 @@
   </sheetPr>
   <dimension ref="B1:J43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>